<commit_message>
Do not include playoff stats
</commit_message>
<xml_diff>
--- a/w26rankings.xlsx
+++ b/w26rankings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sbclaude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71350964-5FE3-4922-8A67-B40C9F8B31A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6142EC8-CB5B-4753-94F6-F840B1A7CDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1358,7 +1358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1368,10 +1368,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1677,14 +1673,11 @@
   <dimension ref="A1:AD165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="28" max="28" width="9.140625" style="8"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1768,7 +1761,7 @@
       <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="7"/>
+      <c r="AB1" s="1"/>
       <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1859,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="AB2" s="3">
-        <f>AC2+Z2</f>
+        <f t="shared" ref="AB2:AB33" si="0">AC2+Z2</f>
         <v>175.1</v>
       </c>
       <c r="AC2" s="3">
@@ -1940,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="AB3" s="3">
-        <f>AC3+Z3</f>
+        <f t="shared" si="0"/>
         <v>169.6</v>
       </c>
       <c r="AC3" s="3">
@@ -2029,7 +2022,7 @@
         <v>1</v>
       </c>
       <c r="AB4" s="3">
-        <f>AC4+Z4</f>
+        <f t="shared" si="0"/>
         <v>156.1</v>
       </c>
       <c r="AC4" s="3">
@@ -2122,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="AB5" s="3">
-        <f>AC5+Z5</f>
+        <f t="shared" si="0"/>
         <v>152.30000000000001</v>
       </c>
       <c r="AC5" s="3">
@@ -2209,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="AB6" s="3">
-        <f>AC6+Z6</f>
+        <f t="shared" si="0"/>
         <v>152.19999999999999</v>
       </c>
       <c r="AC6" s="3">
@@ -2298,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="AB7" s="3">
-        <f>AC7+Z7</f>
+        <f t="shared" si="0"/>
         <v>151.5</v>
       </c>
       <c r="AC7" s="3">
@@ -2391,7 +2384,7 @@
         <v>1</v>
       </c>
       <c r="AB8" s="3">
-        <f>AC8+Z8</f>
+        <f t="shared" si="0"/>
         <v>151.19999999999999</v>
       </c>
       <c r="AC8" s="3">
@@ -2478,7 +2471,7 @@
         <v>2</v>
       </c>
       <c r="AB9" s="3">
-        <f>AC9+Z9</f>
+        <f t="shared" si="0"/>
         <v>147.30000000000001</v>
       </c>
       <c r="AC9" s="3">
@@ -2570,8 +2563,8 @@
       <c r="AA10">
         <v>-2</v>
       </c>
-      <c r="AB10" s="8">
-        <f>AC10+Z10</f>
+      <c r="AB10">
+        <f t="shared" si="0"/>
         <v>143.19999999999999</v>
       </c>
       <c r="AC10">
@@ -2664,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="3">
-        <f>AC11+Z11</f>
+        <f t="shared" si="0"/>
         <v>141.5</v>
       </c>
       <c r="AC11" s="3">
@@ -2751,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="AB12" s="3">
-        <f>AC12+Z12</f>
+        <f t="shared" si="0"/>
         <v>141.30000000000001</v>
       </c>
       <c r="AC12" s="3">
@@ -2844,7 +2837,7 @@
         <v>2</v>
       </c>
       <c r="AB13" s="3">
-        <f>AC13+Z13</f>
+        <f t="shared" si="0"/>
         <v>139.5</v>
       </c>
       <c r="AC13" s="3">
@@ -2923,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="3">
-        <f>AC14+Z14</f>
+        <f t="shared" si="0"/>
         <v>139.19999999999999</v>
       </c>
       <c r="AC14" s="3">
@@ -3007,7 +3000,7 @@
         <v>1</v>
       </c>
       <c r="AB15" s="3">
-        <f>AC15+Z15</f>
+        <f t="shared" si="0"/>
         <v>138.6</v>
       </c>
       <c r="AC15" s="3">
@@ -3100,7 +3093,7 @@
         <v>1</v>
       </c>
       <c r="AB16" s="3">
-        <f>AC16+Z16</f>
+        <f t="shared" si="0"/>
         <v>138.1</v>
       </c>
       <c r="AC16" s="3">
@@ -3187,7 +3180,7 @@
         <v>1</v>
       </c>
       <c r="AB17" s="3">
-        <f>AC17+Z17</f>
+        <f t="shared" si="0"/>
         <v>135.69999999999999</v>
       </c>
       <c r="AC17" s="3">
@@ -3273,8 +3266,8 @@
       <c r="AA18">
         <v>-4</v>
       </c>
-      <c r="AB18" s="8">
-        <f>AC18+Z18</f>
+      <c r="AB18">
+        <f t="shared" si="0"/>
         <v>133.9</v>
       </c>
       <c r="AC18">
@@ -3360,8 +3353,8 @@
       <c r="AA19">
         <v>1</v>
       </c>
-      <c r="AB19" s="8">
-        <f>AC19+Z19</f>
+      <c r="AB19">
+        <f t="shared" si="0"/>
         <v>133</v>
       </c>
       <c r="AC19">
@@ -3450,8 +3443,8 @@
       <c r="AA20">
         <v>2</v>
       </c>
-      <c r="AB20" s="8">
-        <f>AC20+Z20</f>
+      <c r="AB20">
+        <f t="shared" si="0"/>
         <v>132.69999999999999</v>
       </c>
       <c r="AC20">
@@ -3534,8 +3527,8 @@
       <c r="AA21">
         <v>1</v>
       </c>
-      <c r="AB21" s="8">
-        <f>AC21+Z21</f>
+      <c r="AB21">
+        <f t="shared" si="0"/>
         <v>131.19999999999999</v>
       </c>
       <c r="AC21">
@@ -3622,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="AB22" s="3">
-        <f>AC22+Z22</f>
+        <f t="shared" si="0"/>
         <v>130.30000000000001</v>
       </c>
       <c r="AC22" s="3">
@@ -3715,7 +3708,7 @@
         <v>2</v>
       </c>
       <c r="AB23" s="5">
-        <f>AC23+Z23</f>
+        <f t="shared" si="0"/>
         <v>128.80000000000001</v>
       </c>
       <c r="AC23" s="5">
@@ -3801,8 +3794,8 @@
       <c r="AA24">
         <v>-4</v>
       </c>
-      <c r="AB24" s="8">
-        <f>AC24+Z24</f>
+      <c r="AB24">
+        <f t="shared" si="0"/>
         <v>128.5</v>
       </c>
       <c r="AC24">
@@ -3886,101 +3879,101 @@
       <c r="AA25">
         <v>0</v>
       </c>
-      <c r="AB25" s="8">
-        <f>AC25+Z25</f>
+      <c r="AB25">
+        <f t="shared" si="0"/>
         <v>128.30000000000001</v>
       </c>
       <c r="AC25">
         <v>131.30000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>523</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>61</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3">
         <v>70</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="3">
         <v>5</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="3">
         <v>111</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="3">
         <v>128</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="3">
         <v>86.7</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="4">
         <v>0.35099999999999998</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="3">
         <v>39</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="3">
         <v>72</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="4">
         <v>0.314</v>
       </c>
-      <c r="O26" s="2">
+      <c r="O26" s="4">
         <v>0.27400000000000002</v>
       </c>
-      <c r="P26" s="2">
+      <c r="P26" s="4">
         <v>0.318</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="3">
         <v>123</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="3">
         <v>109</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="3">
         <v>123</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="3">
         <v>118.7</v>
       </c>
-      <c r="U26" t="s">
+      <c r="U26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="V26" t="s">
+      <c r="V26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="W26">
+      <c r="W26" s="3">
         <v>100</v>
       </c>
-      <c r="X26">
+      <c r="X26" s="3">
         <v>5</v>
       </c>
-      <c r="Y26">
+      <c r="Y26" s="3">
         <v>3</v>
       </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
-      <c r="AA26">
+      <c r="Z26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="3">
         <v>1</v>
       </c>
-      <c r="AB26" s="8">
-        <f>AC26+Z26</f>
+      <c r="AB26" s="3">
+        <f t="shared" si="0"/>
         <v>127.7</v>
       </c>
-      <c r="AC26">
+      <c r="AC26" s="3">
         <v>127.7</v>
       </c>
     </row>
@@ -4034,7 +4027,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="3">
-        <f>AC27+Z27</f>
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
       <c r="AD27" s="3" t="s">
@@ -4124,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="AB28" s="3">
-        <f>AC28+Z28</f>
+        <f t="shared" si="0"/>
         <v>125.7</v>
       </c>
       <c r="AC28" s="3">
@@ -4216,8 +4209,8 @@
       <c r="AA29">
         <v>0</v>
       </c>
-      <c r="AB29" s="8">
-        <f>AC29+Z29</f>
+      <c r="AB29">
+        <f t="shared" si="0"/>
         <v>124.3</v>
       </c>
       <c r="AC29">
@@ -4303,8 +4296,8 @@
       <c r="AA30">
         <v>2</v>
       </c>
-      <c r="AB30" s="8">
-        <f>AC30+Z30</f>
+      <c r="AB30">
+        <f t="shared" si="0"/>
         <v>122.9</v>
       </c>
       <c r="AC30">
@@ -4390,8 +4383,8 @@
       <c r="AA31">
         <v>1</v>
       </c>
-      <c r="AB31" s="8">
-        <f>AC31+Z31</f>
+      <c r="AB31">
+        <f t="shared" si="0"/>
         <v>122.7</v>
       </c>
       <c r="AC31">
@@ -4451,7 +4444,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="3">
-        <f>AC32+Z32</f>
+        <f t="shared" si="0"/>
         <v>122</v>
       </c>
       <c r="AD32" s="3" t="s">
@@ -4540,8 +4533,8 @@
       <c r="AA33">
         <v>2</v>
       </c>
-      <c r="AB33" s="8">
-        <f>AC33+Z33</f>
+      <c r="AB33">
+        <f t="shared" si="0"/>
         <v>120.9</v>
       </c>
       <c r="AC33">
@@ -4625,7 +4618,7 @@
         <v>0</v>
       </c>
       <c r="AB34" s="3">
-        <f>AC34+Z34</f>
+        <f t="shared" ref="AB34:AB65" si="1">AC34+Z34</f>
         <v>120.8</v>
       </c>
       <c r="AC34" s="3">
@@ -4684,8 +4677,8 @@
       <c r="AA35">
         <v>0</v>
       </c>
-      <c r="AB35" s="8">
-        <f>AC35+Z35</f>
+      <c r="AB35">
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="AD35" t="s">
@@ -4770,8 +4763,8 @@
       <c r="AA36">
         <v>0</v>
       </c>
-      <c r="AB36" s="8">
-        <f>AC36+Z36</f>
+      <c r="AB36">
+        <f t="shared" si="1"/>
         <v>119.1</v>
       </c>
       <c r="AC36">
@@ -4859,8 +4852,8 @@
       <c r="AA37">
         <v>0</v>
       </c>
-      <c r="AB37" s="8">
-        <f>AC37+Z37</f>
+      <c r="AB37">
+        <f t="shared" si="1"/>
         <v>119</v>
       </c>
       <c r="AC37">
@@ -4919,8 +4912,8 @@
       <c r="AA38">
         <v>0</v>
       </c>
-      <c r="AB38" s="8">
-        <f>AC38+Z38</f>
+      <c r="AB38">
+        <f t="shared" si="1"/>
         <v>119</v>
       </c>
       <c r="AD38" t="s">
@@ -5010,7 +5003,7 @@
         <v>2</v>
       </c>
       <c r="AB39" s="5">
-        <f>AC39+Z39</f>
+        <f t="shared" si="1"/>
         <v>118.3</v>
       </c>
       <c r="AC39" s="5">
@@ -5099,7 +5092,7 @@
         <v>1</v>
       </c>
       <c r="AB40" s="5">
-        <f>AC40+Z40</f>
+        <f t="shared" si="1"/>
         <v>118.3</v>
       </c>
       <c r="AC40" s="5">
@@ -5191,8 +5184,8 @@
       <c r="AA41">
         <v>1</v>
       </c>
-      <c r="AB41" s="8">
-        <f>AC41+Z41</f>
+      <c r="AB41">
+        <f t="shared" si="1"/>
         <v>118.1</v>
       </c>
       <c r="AC41">
@@ -5279,7 +5272,7 @@
         <v>0</v>
       </c>
       <c r="AB42" s="3">
-        <f>AC42+Z42</f>
+        <f t="shared" si="1"/>
         <v>117.7</v>
       </c>
       <c r="AC42" s="3">
@@ -5365,8 +5358,8 @@
       <c r="AA43">
         <v>-2</v>
       </c>
-      <c r="AB43" s="8">
-        <f>AC43+Z43</f>
+      <c r="AB43">
+        <f t="shared" si="1"/>
         <v>117.5</v>
       </c>
       <c r="AC43">
@@ -5458,8 +5451,8 @@
       <c r="AA44">
         <v>-2</v>
       </c>
-      <c r="AB44" s="8">
-        <f>AC44+Z44</f>
+      <c r="AB44">
+        <f t="shared" si="1"/>
         <v>117.4</v>
       </c>
       <c r="AC44">
@@ -5546,7 +5539,7 @@
         <v>0</v>
       </c>
       <c r="AB45" s="3">
-        <f>AC45+Z45</f>
+        <f t="shared" si="1"/>
         <v>117.3</v>
       </c>
       <c r="AC45" s="3">
@@ -5632,8 +5625,8 @@
       <c r="AA46">
         <v>1</v>
       </c>
-      <c r="AB46" s="8">
-        <f>AC46+Z46</f>
+      <c r="AB46">
+        <f t="shared" si="1"/>
         <v>117.2</v>
       </c>
       <c r="AC46">
@@ -5722,8 +5715,8 @@
       <c r="AA47">
         <v>0</v>
       </c>
-      <c r="AB47" s="8">
-        <f>AC47+Z47</f>
+      <c r="AB47">
+        <f t="shared" si="1"/>
         <v>116.9</v>
       </c>
       <c r="AC47">
@@ -5809,8 +5802,8 @@
       <c r="AA48">
         <v>-4</v>
       </c>
-      <c r="AB48" s="8">
-        <f>AC48+Z48</f>
+      <c r="AB48">
+        <f t="shared" si="1"/>
         <v>116.9</v>
       </c>
       <c r="AC48">
@@ -5896,8 +5889,8 @@
       <c r="AA49">
         <v>-4</v>
       </c>
-      <c r="AB49" s="8">
-        <f>AC49+Z49</f>
+      <c r="AB49">
+        <f t="shared" si="1"/>
         <v>116.8</v>
       </c>
       <c r="AC49">
@@ -5989,8 +5982,8 @@
       <c r="AA50">
         <v>1</v>
       </c>
-      <c r="AB50" s="8">
-        <f>AC50+Z50</f>
+      <c r="AB50">
+        <f t="shared" si="1"/>
         <v>116.6</v>
       </c>
       <c r="AC50">
@@ -6082,8 +6075,8 @@
       <c r="AA51">
         <v>2</v>
       </c>
-      <c r="AB51" s="8">
-        <f>AC51+Z51</f>
+      <c r="AB51">
+        <f t="shared" si="1"/>
         <v>116.3</v>
       </c>
       <c r="AC51">
@@ -6169,8 +6162,8 @@
       <c r="AA52">
         <v>0</v>
       </c>
-      <c r="AB52" s="8">
-        <f>AC52+Z52</f>
+      <c r="AB52">
+        <f t="shared" si="1"/>
         <v>115.6</v>
       </c>
       <c r="AC52">
@@ -6259,8 +6252,8 @@
       <c r="AA53">
         <v>0</v>
       </c>
-      <c r="AB53" s="8">
-        <f>AC53+Z53</f>
+      <c r="AB53">
+        <f t="shared" si="1"/>
         <v>115.6</v>
       </c>
       <c r="AC53">
@@ -6352,8 +6345,8 @@
       <c r="AA54">
         <v>2</v>
       </c>
-      <c r="AB54" s="8">
-        <f>AC54+Z54</f>
+      <c r="AB54">
+        <f t="shared" si="1"/>
         <v>115.6</v>
       </c>
       <c r="AC54">
@@ -6442,8 +6435,8 @@
       <c r="AA55">
         <v>-2</v>
       </c>
-      <c r="AB55" s="8">
-        <f>AC55+Z55</f>
+      <c r="AB55">
+        <f t="shared" si="1"/>
         <v>115.6</v>
       </c>
       <c r="AC55">
@@ -6535,8 +6528,8 @@
       <c r="AA56">
         <v>2</v>
       </c>
-      <c r="AB56" s="8">
-        <f>AC56+Z56</f>
+      <c r="AB56">
+        <f t="shared" si="1"/>
         <v>115.2</v>
       </c>
       <c r="AC56">
@@ -6606,8 +6599,8 @@
       <c r="AA57">
         <v>0</v>
       </c>
-      <c r="AB57" s="8">
-        <f>AC57+Z57</f>
+      <c r="AB57">
+        <f t="shared" si="1"/>
         <v>115</v>
       </c>
       <c r="AC57"/>
@@ -6685,8 +6678,8 @@
       <c r="AA58">
         <v>0</v>
       </c>
-      <c r="AB58" s="8">
-        <f>AC58+Z58</f>
+      <c r="AB58">
+        <f t="shared" si="1"/>
         <v>114.8</v>
       </c>
       <c r="AC58">
@@ -6769,8 +6762,8 @@
       <c r="AA59">
         <v>1</v>
       </c>
-      <c r="AB59" s="8">
-        <f>AC59+Z59</f>
+      <c r="AB59">
+        <f t="shared" si="1"/>
         <v>114.7</v>
       </c>
       <c r="AC59">
@@ -6850,8 +6843,8 @@
       <c r="AA60">
         <v>2</v>
       </c>
-      <c r="AB60" s="8">
-        <f>AC60+Z60</f>
+      <c r="AB60">
+        <f t="shared" si="1"/>
         <v>114.4</v>
       </c>
       <c r="AC60">
@@ -6937,8 +6930,8 @@
       <c r="AA61">
         <v>1</v>
       </c>
-      <c r="AB61" s="8">
-        <f>AC61+Z61</f>
+      <c r="AB61">
+        <f t="shared" si="1"/>
         <v>113.6</v>
       </c>
       <c r="AC61">
@@ -7031,7 +7024,7 @@
         <v>0</v>
       </c>
       <c r="AB62" s="5">
-        <f>AC62+Z62</f>
+        <f t="shared" si="1"/>
         <v>113.2</v>
       </c>
       <c r="AC62" s="5">
@@ -7120,8 +7113,8 @@
       <c r="AA63">
         <v>-2</v>
       </c>
-      <c r="AB63" s="8">
-        <f>AC63+Z63</f>
+      <c r="AB63">
+        <f t="shared" si="1"/>
         <v>112.6</v>
       </c>
       <c r="AC63">
@@ -7198,8 +7191,8 @@
       <c r="AA64">
         <v>1</v>
       </c>
-      <c r="AB64" s="8">
-        <f>AC64+Z64</f>
+      <c r="AB64">
+        <f t="shared" si="1"/>
         <v>112.4</v>
       </c>
       <c r="AC64">
@@ -7285,8 +7278,8 @@
       <c r="AA65">
         <v>2</v>
       </c>
-      <c r="AB65" s="8">
-        <f>AC65+Z65</f>
+      <c r="AB65">
+        <f t="shared" si="1"/>
         <v>111.9</v>
       </c>
       <c r="AC65">
@@ -7378,8 +7371,8 @@
       <c r="AA66">
         <v>2</v>
       </c>
-      <c r="AB66" s="8">
-        <f>AC66+Z66</f>
+      <c r="AB66">
+        <f t="shared" ref="AB66:AB97" si="2">AC66+Z66</f>
         <v>111.3</v>
       </c>
       <c r="AC66">
@@ -7471,8 +7464,8 @@
       <c r="AA67">
         <v>2</v>
       </c>
-      <c r="AB67" s="8">
-        <f>AC67+Z67</f>
+      <c r="AB67">
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="AC67">
@@ -7564,8 +7557,8 @@
       <c r="AA68">
         <v>1</v>
       </c>
-      <c r="AB68" s="8">
-        <f>AC68+Z68</f>
+      <c r="AB68">
+        <f t="shared" si="2"/>
         <v>109.1</v>
       </c>
       <c r="AC68">
@@ -7650,8 +7643,8 @@
       <c r="AA69">
         <v>0</v>
       </c>
-      <c r="AB69" s="8">
-        <f>AC69+Z69</f>
+      <c r="AB69">
+        <f t="shared" si="2"/>
         <v>109</v>
       </c>
       <c r="AC69">
@@ -7743,8 +7736,8 @@
       <c r="AA70">
         <v>0</v>
       </c>
-      <c r="AB70" s="8">
-        <f>AC70+Z70</f>
+      <c r="AB70">
+        <f t="shared" si="2"/>
         <v>108.9</v>
       </c>
       <c r="AC70">
@@ -7830,8 +7823,8 @@
       <c r="AA71">
         <v>-2</v>
       </c>
-      <c r="AB71" s="8">
-        <f>AC71+Z71</f>
+      <c r="AB71">
+        <f t="shared" si="2"/>
         <v>108.8</v>
       </c>
       <c r="AC71">
@@ -7915,8 +7908,8 @@
       <c r="AA72">
         <v>2</v>
       </c>
-      <c r="AB72" s="8">
-        <f>AC72+Z72</f>
+      <c r="AB72">
+        <f t="shared" si="2"/>
         <v>108.5</v>
       </c>
       <c r="AC72">
@@ -7986,8 +7979,8 @@
       <c r="AA73">
         <v>0</v>
       </c>
-      <c r="AB73" s="8">
-        <f>AC73+Z73</f>
+      <c r="AB73">
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="AC73"/>
@@ -8071,8 +8064,8 @@
       <c r="AA74">
         <v>0</v>
       </c>
-      <c r="AB74" s="8">
-        <f>AC74+Z74</f>
+      <c r="AB74">
+        <f t="shared" si="2"/>
         <v>107.8</v>
       </c>
       <c r="AC74">
@@ -8161,7 +8154,7 @@
         <v>1</v>
       </c>
       <c r="AB75" s="5">
-        <f>AC75+Z75</f>
+        <f t="shared" si="2"/>
         <v>107.5</v>
       </c>
       <c r="AC75" s="5">
@@ -8220,8 +8213,8 @@
       <c r="AA76">
         <v>0</v>
       </c>
-      <c r="AB76" s="8">
-        <f>AC76+Z76</f>
+      <c r="AB76">
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="AD76" t="s">
@@ -8310,8 +8303,8 @@
       <c r="AA77">
         <v>2</v>
       </c>
-      <c r="AB77" s="8">
-        <f>AC77+Z77</f>
+      <c r="AB77">
+        <f t="shared" si="2"/>
         <v>106.5</v>
       </c>
       <c r="AC77">
@@ -8400,8 +8393,8 @@
       <c r="AA78">
         <v>0</v>
       </c>
-      <c r="AB78" s="8">
-        <f>AC78+Z78</f>
+      <c r="AB78">
+        <f t="shared" si="2"/>
         <v>106.4</v>
       </c>
       <c r="AC78">
@@ -8493,8 +8486,8 @@
       <c r="AA79">
         <v>1</v>
       </c>
-      <c r="AB79" s="8">
-        <f>AC79+Z79</f>
+      <c r="AB79">
+        <f t="shared" si="2"/>
         <v>106.2</v>
       </c>
       <c r="AC79">
@@ -8553,8 +8546,8 @@
       <c r="AA80">
         <v>0</v>
       </c>
-      <c r="AB80" s="8">
-        <f>AC80+Z80</f>
+      <c r="AB80">
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="AD80" t="s">
@@ -8644,7 +8637,7 @@
         <v>2</v>
       </c>
       <c r="AB81" s="5">
-        <f>AC81+Z81</f>
+        <f t="shared" si="2"/>
         <v>105.9</v>
       </c>
       <c r="AC81" s="5">
@@ -8735,7 +8728,7 @@
         <v>1</v>
       </c>
       <c r="AB82" s="5">
-        <f>AC82+Z82</f>
+        <f t="shared" si="2"/>
         <v>105.6</v>
       </c>
       <c r="AC82" s="5">
@@ -8815,8 +8808,8 @@
       <c r="AA83">
         <v>1</v>
       </c>
-      <c r="AB83" s="8">
-        <f>AC83+Z83</f>
+      <c r="AB83">
+        <f t="shared" si="2"/>
         <v>105.5</v>
       </c>
       <c r="AC83">
@@ -8905,8 +8898,8 @@
       <c r="AA84">
         <v>1</v>
       </c>
-      <c r="AB84" s="8">
-        <f>AC84+Z84</f>
+      <c r="AB84">
+        <f t="shared" si="2"/>
         <v>105.4</v>
       </c>
       <c r="AC84">
@@ -8986,8 +8979,8 @@
       <c r="AA85">
         <v>2</v>
       </c>
-      <c r="AB85" s="8">
-        <f>AC85+Z85</f>
+      <c r="AB85">
+        <f t="shared" si="2"/>
         <v>105.4</v>
       </c>
       <c r="AC85">
@@ -9080,7 +9073,7 @@
         <v>2</v>
       </c>
       <c r="AB86" s="5">
-        <f>AC86+Z86</f>
+        <f t="shared" si="2"/>
         <v>105.3</v>
       </c>
       <c r="AC86" s="5">
@@ -9164,8 +9157,8 @@
       <c r="AA87">
         <v>-4</v>
       </c>
-      <c r="AB87" s="8">
-        <f>AC87+Z87</f>
+      <c r="AB87">
+        <f t="shared" si="2"/>
         <v>104.8</v>
       </c>
       <c r="AC87">
@@ -9257,8 +9250,8 @@
       <c r="AA88">
         <v>2</v>
       </c>
-      <c r="AB88" s="8">
-        <f>AC88+Z88</f>
+      <c r="AB88">
+        <f t="shared" si="2"/>
         <v>104.4</v>
       </c>
       <c r="AC88">
@@ -9347,8 +9340,8 @@
       <c r="AA89">
         <v>1</v>
       </c>
-      <c r="AB89" s="8">
-        <f>AC89+Z89</f>
+      <c r="AB89">
+        <f t="shared" si="2"/>
         <v>104.4</v>
       </c>
       <c r="AC89">
@@ -9437,8 +9430,8 @@
       <c r="AA90">
         <v>1</v>
       </c>
-      <c r="AB90" s="8">
-        <f>AC90+Z90</f>
+      <c r="AB90">
+        <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="AC90">
@@ -9530,8 +9523,8 @@
       <c r="AA91">
         <v>0</v>
       </c>
-      <c r="AB91" s="8">
-        <f>AC91+Z91</f>
+      <c r="AB91">
+        <f t="shared" si="2"/>
         <v>102.5</v>
       </c>
       <c r="AC91">
@@ -9623,8 +9616,8 @@
       <c r="AA92">
         <v>2</v>
       </c>
-      <c r="AB92" s="8">
-        <f>AC92+Z92</f>
+      <c r="AB92">
+        <f t="shared" si="2"/>
         <v>102.4</v>
       </c>
       <c r="AC92">
@@ -9707,8 +9700,8 @@
       <c r="AA93">
         <v>2</v>
       </c>
-      <c r="AB93" s="8">
-        <f>AC93+Z93</f>
+      <c r="AB93">
+        <f t="shared" si="2"/>
         <v>101.8</v>
       </c>
       <c r="AC93">
@@ -9794,8 +9787,8 @@
       <c r="AA94">
         <v>2</v>
       </c>
-      <c r="AB94" s="8">
-        <f>AC94+Z94</f>
+      <c r="AB94">
+        <f t="shared" si="2"/>
         <v>101.2</v>
       </c>
       <c r="AC94">
@@ -9887,8 +9880,8 @@
       <c r="AA95">
         <v>0</v>
       </c>
-      <c r="AB95" s="8">
-        <f>AC95+Z95</f>
+      <c r="AB95">
+        <f t="shared" si="2"/>
         <v>101</v>
       </c>
       <c r="AC95">
@@ -9977,8 +9970,8 @@
       <c r="AA96">
         <v>0</v>
       </c>
-      <c r="AB96" s="8">
-        <f>AC96+Z96</f>
+      <c r="AB96">
+        <f t="shared" si="2"/>
         <v>100.4</v>
       </c>
       <c r="AC96">
@@ -10058,8 +10051,8 @@
       <c r="AA97">
         <v>1</v>
       </c>
-      <c r="AB97" s="8">
-        <f>AC97+Z97</f>
+      <c r="AB97">
+        <f t="shared" si="2"/>
         <v>100.3</v>
       </c>
       <c r="AC97">
@@ -10151,8 +10144,8 @@
       <c r="AA98">
         <v>1</v>
       </c>
-      <c r="AB98" s="8">
-        <f>AC98+Z98</f>
+      <c r="AB98">
+        <f t="shared" ref="AB98:AB129" si="3">AC98+Z98</f>
         <v>100.2</v>
       </c>
       <c r="AC98">
@@ -10238,8 +10231,8 @@
       <c r="AA99">
         <v>0</v>
       </c>
-      <c r="AB99" s="8">
-        <f>AC99+Z99</f>
+      <c r="AB99">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="AC99">
@@ -10325,8 +10318,8 @@
       <c r="AA100">
         <v>1</v>
       </c>
-      <c r="AB100" s="8">
-        <f>AC100+Z100</f>
+      <c r="AB100">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="AC100">
@@ -10382,8 +10375,8 @@
       <c r="AA101">
         <v>0</v>
       </c>
-      <c r="AB101" s="8">
-        <f>AC101+Z101</f>
+      <c r="AB101">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="AD101" t="s">
@@ -10466,8 +10459,8 @@
       <c r="AA102">
         <v>2</v>
       </c>
-      <c r="AB102" s="8">
-        <f>AC102+Z102</f>
+      <c r="AB102">
+        <f t="shared" si="3"/>
         <v>99.3</v>
       </c>
       <c r="AC102">
@@ -10550,8 +10543,8 @@
       <c r="AA103">
         <v>1</v>
       </c>
-      <c r="AB103" s="8">
-        <f>AC103+Z103</f>
+      <c r="AB103">
+        <f t="shared" si="3"/>
         <v>98.7</v>
       </c>
       <c r="AC103">
@@ -10637,8 +10630,8 @@
       <c r="AA104">
         <v>1</v>
       </c>
-      <c r="AB104" s="8">
-        <f>AC104+Z104</f>
+      <c r="AB104">
+        <f t="shared" si="3"/>
         <v>98.4</v>
       </c>
       <c r="AC104">
@@ -10730,8 +10723,8 @@
       <c r="AA105">
         <v>1</v>
       </c>
-      <c r="AB105" s="8">
-        <f>AC105+Z105</f>
+      <c r="AB105">
+        <f t="shared" si="3"/>
         <v>98.2</v>
       </c>
       <c r="AC105">
@@ -10814,8 +10807,8 @@
       <c r="AA106">
         <v>2</v>
       </c>
-      <c r="AB106" s="8">
-        <f>AC106+Z106</f>
+      <c r="AB106">
+        <f t="shared" si="3"/>
         <v>97.9</v>
       </c>
       <c r="AC106">
@@ -10908,7 +10901,7 @@
         <v>1</v>
       </c>
       <c r="AB107" s="5">
-        <f>AC107+Z107</f>
+        <f t="shared" si="3"/>
         <v>97.3</v>
       </c>
       <c r="AC107" s="5">
@@ -10994,8 +10987,8 @@
       <c r="AA108">
         <v>0</v>
       </c>
-      <c r="AB108" s="8">
-        <f>AC108+Z108</f>
+      <c r="AB108">
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="AC108">
@@ -11087,8 +11080,8 @@
       <c r="AA109">
         <v>2</v>
       </c>
-      <c r="AB109" s="8">
-        <f>AC109+Z109</f>
+      <c r="AB109">
+        <f t="shared" si="3"/>
         <v>96.7</v>
       </c>
       <c r="AC109">
@@ -11177,8 +11170,8 @@
       <c r="AA110">
         <v>1</v>
       </c>
-      <c r="AB110" s="8">
-        <f>AC110+Z110</f>
+      <c r="AB110">
+        <f t="shared" si="3"/>
         <v>96.5</v>
       </c>
       <c r="AC110">
@@ -11270,8 +11263,8 @@
       <c r="AA111">
         <v>1</v>
       </c>
-      <c r="AB111" s="8">
-        <f>AC111+Z111</f>
+      <c r="AB111">
+        <f t="shared" si="3"/>
         <v>96.1</v>
       </c>
       <c r="AC111">
@@ -11361,8 +11354,8 @@
       <c r="AA112">
         <v>2</v>
       </c>
-      <c r="AB112" s="8">
-        <f>AC112+Z112</f>
+      <c r="AB112">
+        <f t="shared" si="3"/>
         <v>95.9</v>
       </c>
       <c r="AC112">
@@ -11448,8 +11441,8 @@
       <c r="AA113">
         <v>-2</v>
       </c>
-      <c r="AB113" s="8">
-        <f>AC113+Z113</f>
+      <c r="AB113">
+        <f t="shared" si="3"/>
         <v>95.4</v>
       </c>
       <c r="AC113">
@@ -11529,8 +11522,8 @@
       <c r="AA114">
         <v>2</v>
       </c>
-      <c r="AB114" s="8">
-        <f>AC114+Z114</f>
+      <c r="AB114">
+        <f t="shared" si="3"/>
         <v>95.3</v>
       </c>
       <c r="AC114">
@@ -11589,8 +11582,8 @@
       <c r="AA115">
         <v>0</v>
       </c>
-      <c r="AB115" s="8">
-        <f>AC115+Z115</f>
+      <c r="AB115">
+        <f t="shared" si="3"/>
         <v>95</v>
       </c>
       <c r="AD115" t="s">
@@ -11673,8 +11666,8 @@
       <c r="AA116">
         <v>2</v>
       </c>
-      <c r="AB116" s="8">
-        <f>AC116+Z116</f>
+      <c r="AB116">
+        <f t="shared" si="3"/>
         <v>94.5</v>
       </c>
       <c r="AC116">
@@ -11757,8 +11750,8 @@
       <c r="AA117">
         <v>1</v>
       </c>
-      <c r="AB117" s="8">
-        <f>AC117+Z117</f>
+      <c r="AB117">
+        <f t="shared" si="3"/>
         <v>94.5</v>
       </c>
       <c r="AC117">
@@ -11841,8 +11834,8 @@
       <c r="AA118">
         <v>0</v>
       </c>
-      <c r="AB118" s="8">
-        <f>AC118+Z118</f>
+      <c r="AB118">
+        <f t="shared" si="3"/>
         <v>93.9</v>
       </c>
       <c r="AC118">
@@ -11928,8 +11921,8 @@
       <c r="AA119">
         <v>2</v>
       </c>
-      <c r="AB119" s="8">
-        <f>AC119+Z119</f>
+      <c r="AB119">
+        <f t="shared" si="3"/>
         <v>93.3</v>
       </c>
       <c r="AC119">
@@ -12016,7 +12009,7 @@
         <v>1</v>
       </c>
       <c r="AB120" s="5">
-        <f>AC120+Z120</f>
+        <f t="shared" si="3"/>
         <v>92.8</v>
       </c>
       <c r="AC120" s="5">
@@ -12102,8 +12095,8 @@
       <c r="AA121">
         <v>1</v>
       </c>
-      <c r="AB121" s="8">
-        <f>AC121+Z121</f>
+      <c r="AB121">
+        <f t="shared" si="3"/>
         <v>92.6</v>
       </c>
       <c r="AC121">
@@ -12186,8 +12179,8 @@
       <c r="AA122">
         <v>1</v>
       </c>
-      <c r="AB122" s="8">
-        <f>AC122+Z122</f>
+      <c r="AB122">
+        <f t="shared" si="3"/>
         <v>91.9</v>
       </c>
       <c r="AC122">
@@ -12273,8 +12266,8 @@
       <c r="AA123">
         <v>-4</v>
       </c>
-      <c r="AB123" s="8">
-        <f>AC123+Z123</f>
+      <c r="AB123">
+        <f t="shared" si="3"/>
         <v>91.8</v>
       </c>
       <c r="AC123">
@@ -12366,8 +12359,8 @@
       <c r="AA124">
         <v>2</v>
       </c>
-      <c r="AB124" s="8">
-        <f>AC124+Z124</f>
+      <c r="AB124">
+        <f t="shared" si="3"/>
         <v>91.8</v>
       </c>
       <c r="AC124">
@@ -12450,8 +12443,8 @@
       <c r="AA125">
         <v>-4</v>
       </c>
-      <c r="AB125" s="8">
-        <f>AC125+Z125</f>
+      <c r="AB125">
+        <f t="shared" si="3"/>
         <v>91.3</v>
       </c>
       <c r="AC125">
@@ -12543,8 +12536,8 @@
       <c r="AA126">
         <v>2</v>
       </c>
-      <c r="AB126" s="8">
-        <f>AC126+Z126</f>
+      <c r="AB126">
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="AC126">
@@ -12627,8 +12620,8 @@
       <c r="AA127">
         <v>2</v>
       </c>
-      <c r="AB127" s="8">
-        <f>AC127+Z127</f>
+      <c r="AB127">
+        <f t="shared" si="3"/>
         <v>90.9</v>
       </c>
       <c r="AC127">
@@ -12714,8 +12707,8 @@
       <c r="AA128">
         <v>1</v>
       </c>
-      <c r="AB128" s="8">
-        <f>AC128+Z128</f>
+      <c r="AB128">
+        <f t="shared" si="3"/>
         <v>90.9</v>
       </c>
       <c r="AC128">
@@ -12807,8 +12800,8 @@
       <c r="AA129">
         <v>1</v>
       </c>
-      <c r="AB129" s="8">
-        <f>AC129+Z129</f>
+      <c r="AB129">
+        <f t="shared" si="3"/>
         <v>90.2</v>
       </c>
       <c r="AC129">
@@ -12901,7 +12894,7 @@
         <v>2</v>
       </c>
       <c r="AB130" s="5">
-        <f>AC130+Z130</f>
+        <f t="shared" ref="AB130:AB161" si="4">AC130+Z130</f>
         <v>90.2</v>
       </c>
       <c r="AC130" s="5">
@@ -12993,8 +12986,8 @@
       <c r="AA131">
         <v>0</v>
       </c>
-      <c r="AB131" s="8">
-        <f>AC131+Z131</f>
+      <c r="AB131">
+        <f t="shared" si="4"/>
         <v>89.4</v>
       </c>
       <c r="AC131">
@@ -13077,8 +13070,8 @@
       <c r="AA132">
         <v>0</v>
       </c>
-      <c r="AB132" s="8">
-        <f>AC132+Z132</f>
+      <c r="AB132">
+        <f t="shared" si="4"/>
         <v>88.5</v>
       </c>
       <c r="AC132">
@@ -13164,8 +13157,8 @@
       <c r="AA133">
         <v>-4</v>
       </c>
-      <c r="AB133" s="8">
-        <f>AC133+Z133</f>
+      <c r="AB133">
+        <f t="shared" si="4"/>
         <v>88.4</v>
       </c>
       <c r="AC133">
@@ -13257,8 +13250,8 @@
       <c r="AA134">
         <v>1</v>
       </c>
-      <c r="AB134" s="8">
-        <f>AC134+Z134</f>
+      <c r="AB134">
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="AC134">
@@ -13347,8 +13340,8 @@
       <c r="AA135">
         <v>1</v>
       </c>
-      <c r="AB135" s="8">
-        <f>AC135+Z135</f>
+      <c r="AB135">
+        <f t="shared" si="4"/>
         <v>86.7</v>
       </c>
       <c r="AC135">
@@ -13431,8 +13424,8 @@
       <c r="AA136">
         <v>0</v>
       </c>
-      <c r="AB136" s="8">
-        <f>AC136+Z136</f>
+      <c r="AB136">
+        <f t="shared" si="4"/>
         <v>86.4</v>
       </c>
       <c r="AC136">
@@ -13518,8 +13511,8 @@
       <c r="AA137">
         <v>-2</v>
       </c>
-      <c r="AB137" s="8">
-        <f>AC137+Z137</f>
+      <c r="AB137">
+        <f t="shared" si="4"/>
         <v>86.4</v>
       </c>
       <c r="AC137">
@@ -13611,8 +13604,8 @@
       <c r="AA138">
         <v>1</v>
       </c>
-      <c r="AB138" s="8">
-        <f>AC138+Z138</f>
+      <c r="AB138">
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="AC138">
@@ -13695,8 +13688,8 @@
       <c r="AA139">
         <v>0</v>
       </c>
-      <c r="AB139" s="8">
-        <f>AC139+Z139</f>
+      <c r="AB139">
+        <f t="shared" si="4"/>
         <v>84.7</v>
       </c>
       <c r="AC139">
@@ -13782,8 +13775,8 @@
       <c r="AA140">
         <v>2</v>
       </c>
-      <c r="AB140" s="8">
-        <f>AC140+Z140</f>
+      <c r="AB140">
+        <f t="shared" si="4"/>
         <v>84.3</v>
       </c>
       <c r="AC140">
@@ -13869,8 +13862,8 @@
       <c r="AA141">
         <v>0</v>
       </c>
-      <c r="AB141" s="8">
-        <f>AC141+Z141</f>
+      <c r="AB141">
+        <f t="shared" si="4"/>
         <v>84.3</v>
       </c>
       <c r="AC141">
@@ -13956,8 +13949,8 @@
       <c r="AA142">
         <v>2</v>
       </c>
-      <c r="AB142" s="8">
-        <f>AC142+Z142</f>
+      <c r="AB142">
+        <f t="shared" si="4"/>
         <v>84.1</v>
       </c>
       <c r="AC142">
@@ -14046,8 +14039,8 @@
       <c r="AA143">
         <v>2</v>
       </c>
-      <c r="AB143" s="8">
-        <f>AC143+Z143</f>
+      <c r="AB143">
+        <f t="shared" si="4"/>
         <v>83.9</v>
       </c>
       <c r="AC143">
@@ -14139,8 +14132,8 @@
       <c r="AA144">
         <v>2</v>
       </c>
-      <c r="AB144" s="8">
-        <f>AC144+Z144</f>
+      <c r="AB144">
+        <f t="shared" si="4"/>
         <v>83.9</v>
       </c>
       <c r="AC144">
@@ -14232,8 +14225,8 @@
       <c r="AA145">
         <v>2</v>
       </c>
-      <c r="AB145" s="8">
-        <f>AC145+Z145</f>
+      <c r="AB145">
+        <f t="shared" si="4"/>
         <v>83.8</v>
       </c>
       <c r="AC145">
@@ -14325,8 +14318,8 @@
       <c r="AA146">
         <v>1</v>
       </c>
-      <c r="AB146" s="8">
-        <f>AC146+Z146</f>
+      <c r="AB146">
+        <f t="shared" si="4"/>
         <v>83.5</v>
       </c>
       <c r="AC146">
@@ -14412,8 +14405,8 @@
       <c r="AA147">
         <v>2</v>
       </c>
-      <c r="AB147" s="8">
-        <f>AC147+Z147</f>
+      <c r="AB147">
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="AC147">
@@ -14502,8 +14495,8 @@
       <c r="AA148">
         <v>2</v>
       </c>
-      <c r="AB148" s="8">
-        <f>AC148+Z148</f>
+      <c r="AB148">
+        <f t="shared" si="4"/>
         <v>81.5</v>
       </c>
       <c r="AC148">
@@ -14586,8 +14579,8 @@
       <c r="AA149">
         <v>0</v>
       </c>
-      <c r="AB149" s="8">
-        <f>AC149+Z149</f>
+      <c r="AB149">
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="AC149">
@@ -14679,8 +14672,8 @@
       <c r="AA150">
         <v>1</v>
       </c>
-      <c r="AB150" s="8">
-        <f>AC150+Z150</f>
+      <c r="AB150">
+        <f t="shared" si="4"/>
         <v>80.099999999999994</v>
       </c>
       <c r="AC150">
@@ -14766,8 +14759,8 @@
       <c r="AA151">
         <v>0</v>
       </c>
-      <c r="AB151" s="8">
-        <f>AC151+Z151</f>
+      <c r="AB151">
+        <f t="shared" si="4"/>
         <v>77.900000000000006</v>
       </c>
       <c r="AC151">
@@ -14859,8 +14852,8 @@
       <c r="AA152">
         <v>0</v>
       </c>
-      <c r="AB152" s="8">
-        <f>AC152+Z152</f>
+      <c r="AB152">
+        <f t="shared" si="4"/>
         <v>77.599999999999994</v>
       </c>
       <c r="AC152">
@@ -14950,7 +14943,7 @@
         <v>1</v>
       </c>
       <c r="AB153" s="5">
-        <f>AC153+Z153</f>
+        <f t="shared" si="4"/>
         <v>76.8</v>
       </c>
       <c r="AC153" s="5">
@@ -15042,8 +15035,8 @@
       <c r="AA154">
         <v>2</v>
       </c>
-      <c r="AB154" s="8">
-        <f>AC154+Z154</f>
+      <c r="AB154">
+        <f t="shared" si="4"/>
         <v>76.400000000000006</v>
       </c>
       <c r="AC154">
@@ -15135,8 +15128,8 @@
       <c r="AA155">
         <v>0</v>
       </c>
-      <c r="AB155" s="8">
-        <f>AC155+Z155</f>
+      <c r="AB155">
+        <f t="shared" si="4"/>
         <v>76.3</v>
       </c>
       <c r="AC155">
@@ -15228,8 +15221,8 @@
       <c r="AA156">
         <v>2</v>
       </c>
-      <c r="AB156" s="8">
-        <f>AC156+Z156</f>
+      <c r="AB156">
+        <f t="shared" si="4"/>
         <v>75.5</v>
       </c>
       <c r="AC156">
@@ -15315,8 +15308,8 @@
       <c r="AA157">
         <v>1</v>
       </c>
-      <c r="AB157" s="8">
-        <f>AC157+Z157</f>
+      <c r="AB157">
+        <f t="shared" si="4"/>
         <v>75.3</v>
       </c>
       <c r="AC157">
@@ -15408,8 +15401,8 @@
       <c r="AA158">
         <v>2</v>
       </c>
-      <c r="AB158" s="8">
-        <f>AC158+Z158</f>
+      <c r="AB158">
+        <f t="shared" si="4"/>
         <v>75.2</v>
       </c>
       <c r="AC158">
@@ -15501,8 +15494,8 @@
       <c r="AA159">
         <v>1</v>
       </c>
-      <c r="AB159" s="8">
-        <f>AC159+Z159</f>
+      <c r="AB159">
+        <f t="shared" si="4"/>
         <v>74.8</v>
       </c>
       <c r="AC159">
@@ -15591,8 +15584,8 @@
       <c r="AA160">
         <v>2</v>
       </c>
-      <c r="AB160" s="8">
-        <f>AC160+Z160</f>
+      <c r="AB160">
+        <f t="shared" si="4"/>
         <v>72.900000000000006</v>
       </c>
       <c r="AC160">
@@ -15678,8 +15671,8 @@
       <c r="AA161">
         <v>0</v>
       </c>
-      <c r="AB161" s="8">
-        <f>AC161+Z161</f>
+      <c r="AB161">
+        <f t="shared" si="4"/>
         <v>72.900000000000006</v>
       </c>
       <c r="AC161">
@@ -15762,8 +15755,8 @@
       <c r="AA162">
         <v>1</v>
       </c>
-      <c r="AB162" s="8">
-        <f>AC162+Z162</f>
+      <c r="AB162">
+        <f t="shared" ref="AB162:AB193" si="5">AC162+Z162</f>
         <v>72</v>
       </c>
       <c r="AC162">
@@ -15852,8 +15845,8 @@
       <c r="AA163">
         <v>1</v>
       </c>
-      <c r="AB163" s="8">
-        <f>AC163+Z163</f>
+      <c r="AB163">
+        <f t="shared" si="5"/>
         <v>66.5</v>
       </c>
       <c r="AC163">
@@ -15946,7 +15939,7 @@
         <v>1</v>
       </c>
       <c r="AB164" s="5">
-        <f>AC164+Z164</f>
+        <f t="shared" si="5"/>
         <v>60.2</v>
       </c>
       <c r="AC164" s="5">
@@ -16026,8 +16019,8 @@
       <c r="AA165">
         <v>1</v>
       </c>
-      <c r="AB165" s="8">
-        <f>AC165+Z165</f>
+      <c r="AB165">
+        <f t="shared" si="5"/>
         <v>-99896.2</v>
       </c>
       <c r="AC165">

</xml_diff>

<commit_message>
Change W26 Division Name
</commit_message>
<xml_diff>
--- a/w26rankings.xlsx
+++ b/w26rankings.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sbclaude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EDBF7F-A186-40DF-A7FB-40547A1EACC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F45B86-30F7-4F2B-9A17-55F3F5899D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rankings" sheetId="1" r:id="rId1"/>
-    <sheet name="Teams" sheetId="4" r:id="rId2"/>
-    <sheet name="Contact_Info" sheetId="3" r:id="rId3"/>
-    <sheet name="Summary" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="Teams" sheetId="4" r:id="rId3"/>
+    <sheet name="Contact_Info" sheetId="3" r:id="rId4"/>
+    <sheet name="Summary" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3496" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4011" uniqueCount="973">
   <si>
     <t>PID</t>
   </si>
@@ -2978,13 +2979,44 @@
   <si>
     <t>L</t>
   </si>
+  <si>
+    <t>Wolverines</t>
+  </si>
+  <si>
+    <t>Norsemen</t>
+  </si>
+  <si>
+    <t>Xtreme</t>
+  </si>
+  <si>
+    <t>Buckeyes</t>
+  </si>
+  <si>
+    <t>Rebels</t>
+  </si>
+  <si>
+    <t>Gunslingers</t>
+  </si>
+  <si>
+    <t>Tigers</t>
+  </si>
+  <si>
+    <t>Shorebirds</t>
+  </si>
+  <si>
+    <t>Bearcats</t>
+  </si>
+  <si>
+    <t>DEATHSTARS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode=".000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -3068,7 +3100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3092,6 +3124,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3459,8 +3492,8 @@
   <dimension ref="A1:AG165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B137" sqref="B137"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19437,11 +19470,2538 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841198FB-CC6C-47EF-8254-9DC59DADECA3}">
+  <dimension ref="A1:L165"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>946</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>791</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
+        <v>802</v>
+      </c>
+      <c r="J2" t="s">
+        <v>963</v>
+      </c>
+      <c r="K2" s="13">
+        <f>AVERAGEIF(A:A,I2,D:D)</f>
+        <v>61.272727272727273</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIFS(A:A,I2,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>796</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>58</v>
+      </c>
+      <c r="I3" t="s">
+        <v>792</v>
+      </c>
+      <c r="J3" t="s">
+        <v>968</v>
+      </c>
+      <c r="K3" s="13">
+        <f>AVERAGEIF(A:A,I3,D:D)</f>
+        <v>61.636363636363633</v>
+      </c>
+      <c r="L3">
+        <f>COUNTIFS(A:A,I3,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>793</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>795</v>
+      </c>
+      <c r="J4" t="s">
+        <v>795</v>
+      </c>
+      <c r="K4" s="13">
+        <f>AVERAGEIF(A:A,I4,D:D)</f>
+        <v>61.727272727272727</v>
+      </c>
+      <c r="L4">
+        <f>COUNTIFS(A:A,I4,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>795</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5">
+        <v>55</v>
+      </c>
+      <c r="I5" t="s">
+        <v>797</v>
+      </c>
+      <c r="J5" t="s">
+        <v>964</v>
+      </c>
+      <c r="K5" s="13">
+        <f>AVERAGEIF(A:A,I5,D:D)</f>
+        <v>62.18181818181818</v>
+      </c>
+      <c r="L5">
+        <f>COUNTIFS(A:A,I5,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>800</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>58</v>
+      </c>
+      <c r="I6" t="s">
+        <v>801</v>
+      </c>
+      <c r="J6" t="s">
+        <v>970</v>
+      </c>
+      <c r="K6" s="13">
+        <f>AVERAGEIF(A:A,I6,D:D)</f>
+        <v>62.272727272727273</v>
+      </c>
+      <c r="L6">
+        <f>COUNTIFS(A:A,I6,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>792</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7">
+        <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>800</v>
+      </c>
+      <c r="J7" t="s">
+        <v>965</v>
+      </c>
+      <c r="K7" s="13">
+        <f>AVERAGEIF(A:A,I7,D:D)</f>
+        <v>62.727272727272727</v>
+      </c>
+      <c r="L7">
+        <f>COUNTIFS(A:A,I7,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>794</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>790</v>
+      </c>
+      <c r="J8" t="s">
+        <v>790</v>
+      </c>
+      <c r="K8" s="13">
+        <f>AVERAGEIF(A:A,I8,D:D)</f>
+        <v>62.81818181818182</v>
+      </c>
+      <c r="L8">
+        <f>COUNTIFS(A:A,I8,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>797</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9">
+        <v>68</v>
+      </c>
+      <c r="I9" t="s">
+        <v>794</v>
+      </c>
+      <c r="J9" t="s">
+        <v>969</v>
+      </c>
+      <c r="K9" s="13">
+        <f>AVERAGEIF(A:A,I9,D:D)</f>
+        <v>62.909090909090907</v>
+      </c>
+      <c r="L9">
+        <f>COUNTIFS(A:A,I9,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>794</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10">
+        <v>63</v>
+      </c>
+      <c r="I10" t="s">
+        <v>791</v>
+      </c>
+      <c r="J10" t="s">
+        <v>791</v>
+      </c>
+      <c r="K10" s="13">
+        <f>AVERAGEIF(A:A,I10,D:D)</f>
+        <v>63</v>
+      </c>
+      <c r="L10">
+        <f>COUNTIFS(A:A,I10,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>802</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11">
+        <v>62</v>
+      </c>
+      <c r="I11" t="s">
+        <v>798</v>
+      </c>
+      <c r="J11" t="s">
+        <v>966</v>
+      </c>
+      <c r="K11" s="13">
+        <f>AVERAGEIF(A:A,I11,D:D)</f>
+        <v>63.545454545454547</v>
+      </c>
+      <c r="L11">
+        <f>COUNTIFS(A:A,I11,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>797</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12">
+        <v>60</v>
+      </c>
+      <c r="I12" t="s">
+        <v>799</v>
+      </c>
+      <c r="J12" t="s">
+        <v>799</v>
+      </c>
+      <c r="K12" s="13">
+        <f>AVERAGEIF(A:A,I12,D:D)</f>
+        <v>64.272727272727266</v>
+      </c>
+      <c r="L12">
+        <f>COUNTIFS(A:A,I12,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>790</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13">
+        <v>54</v>
+      </c>
+      <c r="I13" t="s">
+        <v>796</v>
+      </c>
+      <c r="J13" t="s">
+        <v>972</v>
+      </c>
+      <c r="K13" s="13">
+        <f>AVERAGEIF(A:A,I13,D:D)</f>
+        <v>64.818181818181813</v>
+      </c>
+      <c r="L13">
+        <f>COUNTIFS(A:A,I13,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>802</v>
+      </c>
+      <c r="B14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>793</v>
+      </c>
+      <c r="J14" t="s">
+        <v>967</v>
+      </c>
+      <c r="K14" s="13">
+        <f>AVERAGEIF(A:A,I14,D:D)</f>
+        <v>65.090909090909093</v>
+      </c>
+      <c r="L14">
+        <f>COUNTIFS(A:A,I14,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>799</v>
+      </c>
+      <c r="B15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>803</v>
+      </c>
+      <c r="J15" t="s">
+        <v>971</v>
+      </c>
+      <c r="K15" s="13">
+        <f>AVERAGEIF(A:A,I15,D:D)</f>
+        <v>65.454545454545453</v>
+      </c>
+      <c r="L15">
+        <f>COUNTIFS(A:A,I15,D:D,"&gt;0")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>801</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>796</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>803</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>799</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>792</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>791</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>801</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>792</v>
+      </c>
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>793</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>793</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>795</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>803</v>
+      </c>
+      <c r="B27" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" t="s">
+        <v>401</v>
+      </c>
+      <c r="D27">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>800</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>797</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>790</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>803</v>
+      </c>
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>803</v>
+      </c>
+      <c r="B32" t="s">
+        <v>351</v>
+      </c>
+      <c r="C32" t="s">
+        <v>406</v>
+      </c>
+      <c r="D32">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>802</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>799</v>
+      </c>
+      <c r="B34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>802</v>
+      </c>
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" t="s">
+        <v>408</v>
+      </c>
+      <c r="D35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>790</v>
+      </c>
+      <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>794</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>802</v>
+      </c>
+      <c r="B38" t="s">
+        <v>399</v>
+      </c>
+      <c r="C38" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>796</v>
+      </c>
+      <c r="B39" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>794</v>
+      </c>
+      <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>793</v>
+      </c>
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>798</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>150</v>
+      </c>
+      <c r="D42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>794</v>
+      </c>
+      <c r="B43" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>796</v>
+      </c>
+      <c r="B44" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>798</v>
+      </c>
+      <c r="B45" t="s">
+        <v>158</v>
+      </c>
+      <c r="C45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>792</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>791</v>
+      </c>
+      <c r="B47" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>791</v>
+      </c>
+      <c r="B48" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>795</v>
+      </c>
+      <c r="B49" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>796</v>
+      </c>
+      <c r="B50" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" t="s">
+        <v>166</v>
+      </c>
+      <c r="D50">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>790</v>
+      </c>
+      <c r="B51" t="s">
+        <v>183</v>
+      </c>
+      <c r="C51" t="s">
+        <v>184</v>
+      </c>
+      <c r="D51">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>800</v>
+      </c>
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" t="s">
+        <v>174</v>
+      </c>
+      <c r="D52">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>791</v>
+      </c>
+      <c r="B53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>792</v>
+      </c>
+      <c r="B54" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>798</v>
+      </c>
+      <c r="B55" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>792</v>
+      </c>
+      <c r="B56" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>802</v>
+      </c>
+      <c r="B57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" t="s">
+        <v>306</v>
+      </c>
+      <c r="D57">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>803</v>
+      </c>
+      <c r="B58" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" t="s">
+        <v>188</v>
+      </c>
+      <c r="D58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>794</v>
+      </c>
+      <c r="B59" t="s">
+        <v>169</v>
+      </c>
+      <c r="C59" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>793</v>
+      </c>
+      <c r="B60" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" t="s">
+        <v>191</v>
+      </c>
+      <c r="D60">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>790</v>
+      </c>
+      <c r="B61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" t="s">
+        <v>198</v>
+      </c>
+      <c r="D61">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>800</v>
+      </c>
+      <c r="B62" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>800</v>
+      </c>
+      <c r="B63" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>795</v>
+      </c>
+      <c r="B64" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>799</v>
+      </c>
+      <c r="B65" t="s">
+        <v>35</v>
+      </c>
+      <c r="C65" t="s">
+        <v>202</v>
+      </c>
+      <c r="D65">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>797</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" t="s">
+        <v>198</v>
+      </c>
+      <c r="D66">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>803</v>
+      </c>
+      <c r="B67" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>803</v>
+      </c>
+      <c r="B68" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>801</v>
+      </c>
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" t="s">
+        <v>213</v>
+      </c>
+      <c r="D69">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>795</v>
+      </c>
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" t="s">
+        <v>138</v>
+      </c>
+      <c r="D70">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>791</v>
+      </c>
+      <c r="B71" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" t="s">
+        <v>209</v>
+      </c>
+      <c r="D71">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>800</v>
+      </c>
+      <c r="B72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" t="s">
+        <v>211</v>
+      </c>
+      <c r="D72">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>802</v>
+      </c>
+      <c r="B73" t="s">
+        <v>123</v>
+      </c>
+      <c r="C73" t="s">
+        <v>402</v>
+      </c>
+      <c r="D73">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>797</v>
+      </c>
+      <c r="B74" t="s">
+        <v>215</v>
+      </c>
+      <c r="C74" t="s">
+        <v>216</v>
+      </c>
+      <c r="D74">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>798</v>
+      </c>
+      <c r="B75" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>802</v>
+      </c>
+      <c r="B76" t="s">
+        <v>215</v>
+      </c>
+      <c r="C76" t="s">
+        <v>404</v>
+      </c>
+      <c r="D76">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>793</v>
+      </c>
+      <c r="B77" t="s">
+        <v>221</v>
+      </c>
+      <c r="C77" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>801</v>
+      </c>
+      <c r="B78" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" t="s">
+        <v>236</v>
+      </c>
+      <c r="D78">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>800</v>
+      </c>
+      <c r="B79" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" t="s">
+        <v>223</v>
+      </c>
+      <c r="D79">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>795</v>
+      </c>
+      <c r="B80" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" t="s">
+        <v>395</v>
+      </c>
+      <c r="D80">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>802</v>
+      </c>
+      <c r="B81" t="s">
+        <v>225</v>
+      </c>
+      <c r="C81" t="s">
+        <v>226</v>
+      </c>
+      <c r="D81">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>797</v>
+      </c>
+      <c r="B82" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" t="s">
+        <v>227</v>
+      </c>
+      <c r="D82">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>801</v>
+      </c>
+      <c r="B83" t="s">
+        <v>51</v>
+      </c>
+      <c r="C83" t="s">
+        <v>228</v>
+      </c>
+      <c r="D83">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>798</v>
+      </c>
+      <c r="B84" t="s">
+        <v>230</v>
+      </c>
+      <c r="C84" t="s">
+        <v>231</v>
+      </c>
+      <c r="D84">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>791</v>
+      </c>
+      <c r="B85" t="s">
+        <v>233</v>
+      </c>
+      <c r="C85" t="s">
+        <v>234</v>
+      </c>
+      <c r="D85">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>799</v>
+      </c>
+      <c r="B86" t="s">
+        <v>112</v>
+      </c>
+      <c r="C86" t="s">
+        <v>238</v>
+      </c>
+      <c r="D86">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>796</v>
+      </c>
+      <c r="B87" t="s">
+        <v>248</v>
+      </c>
+      <c r="C87" t="s">
+        <v>249</v>
+      </c>
+      <c r="D87">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>801</v>
+      </c>
+      <c r="B88" t="s">
+        <v>137</v>
+      </c>
+      <c r="C88" t="s">
+        <v>239</v>
+      </c>
+      <c r="D88">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>791</v>
+      </c>
+      <c r="B89" t="s">
+        <v>104</v>
+      </c>
+      <c r="C89" t="s">
+        <v>240</v>
+      </c>
+      <c r="D89">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>800</v>
+      </c>
+      <c r="B90" t="s">
+        <v>245</v>
+      </c>
+      <c r="C90" t="s">
+        <v>246</v>
+      </c>
+      <c r="D90">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>794</v>
+      </c>
+      <c r="B91" t="s">
+        <v>46</v>
+      </c>
+      <c r="C91" t="s">
+        <v>255</v>
+      </c>
+      <c r="D91">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>796</v>
+      </c>
+      <c r="B92" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" t="s">
+        <v>257</v>
+      </c>
+      <c r="D92">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>801</v>
+      </c>
+      <c r="B93" t="s">
+        <v>258</v>
+      </c>
+      <c r="C93" t="s">
+        <v>259</v>
+      </c>
+      <c r="D93">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>794</v>
+      </c>
+      <c r="B94" t="s">
+        <v>158</v>
+      </c>
+      <c r="C94" t="s">
+        <v>263</v>
+      </c>
+      <c r="D94">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>798</v>
+      </c>
+      <c r="B95" t="s">
+        <v>265</v>
+      </c>
+      <c r="C95" t="s">
+        <v>266</v>
+      </c>
+      <c r="D95">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>792</v>
+      </c>
+      <c r="B96" t="s">
+        <v>261</v>
+      </c>
+      <c r="C96" t="s">
+        <v>262</v>
+      </c>
+      <c r="D96">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>792</v>
+      </c>
+      <c r="B97" t="s">
+        <v>241</v>
+      </c>
+      <c r="C97" t="s">
+        <v>242</v>
+      </c>
+      <c r="D97">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>801</v>
+      </c>
+      <c r="B98" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98" t="s">
+        <v>270</v>
+      </c>
+      <c r="D98">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>790</v>
+      </c>
+      <c r="B99" t="s">
+        <v>29</v>
+      </c>
+      <c r="C99" t="s">
+        <v>267</v>
+      </c>
+      <c r="D99">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>796</v>
+      </c>
+      <c r="B100" t="s">
+        <v>98</v>
+      </c>
+      <c r="C100" t="s">
+        <v>285</v>
+      </c>
+      <c r="D100">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>791</v>
+      </c>
+      <c r="B101" t="s">
+        <v>120</v>
+      </c>
+      <c r="C101" t="s">
+        <v>411</v>
+      </c>
+      <c r="D101">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>800</v>
+      </c>
+      <c r="B102" t="s">
+        <v>66</v>
+      </c>
+      <c r="C102" t="s">
+        <v>272</v>
+      </c>
+      <c r="D102">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>798</v>
+      </c>
+      <c r="B103" t="s">
+        <v>273</v>
+      </c>
+      <c r="C103" t="s">
+        <v>274</v>
+      </c>
+      <c r="D103">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>795</v>
+      </c>
+      <c r="B104" t="s">
+        <v>169</v>
+      </c>
+      <c r="C104" t="s">
+        <v>280</v>
+      </c>
+      <c r="D104">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>796</v>
+      </c>
+      <c r="B105" t="s">
+        <v>276</v>
+      </c>
+      <c r="C105" t="s">
+        <v>277</v>
+      </c>
+      <c r="D105">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>797</v>
+      </c>
+      <c r="B106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C106" t="s">
+        <v>278</v>
+      </c>
+      <c r="D106">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>790</v>
+      </c>
+      <c r="B107" t="s">
+        <v>282</v>
+      </c>
+      <c r="C107" t="s">
+        <v>283</v>
+      </c>
+      <c r="D107">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>790</v>
+      </c>
+      <c r="B108" t="s">
+        <v>294</v>
+      </c>
+      <c r="C108" t="s">
+        <v>295</v>
+      </c>
+      <c r="D108">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>797</v>
+      </c>
+      <c r="B109" t="s">
+        <v>286</v>
+      </c>
+      <c r="C109" t="s">
+        <v>287</v>
+      </c>
+      <c r="D109">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>793</v>
+      </c>
+      <c r="B110" t="s">
+        <v>289</v>
+      </c>
+      <c r="C110" t="s">
+        <v>290</v>
+      </c>
+      <c r="D110">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>792</v>
+      </c>
+      <c r="B111" t="s">
+        <v>292</v>
+      </c>
+      <c r="C111" t="s">
+        <v>293</v>
+      </c>
+      <c r="D111">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>795</v>
+      </c>
+      <c r="B112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C112" t="s">
+        <v>298</v>
+      </c>
+      <c r="D112">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>801</v>
+      </c>
+      <c r="B113" t="s">
+        <v>276</v>
+      </c>
+      <c r="C113" t="s">
+        <v>304</v>
+      </c>
+      <c r="D113">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>796</v>
+      </c>
+      <c r="B114" t="s">
+        <v>169</v>
+      </c>
+      <c r="C114" t="s">
+        <v>300</v>
+      </c>
+      <c r="D114">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>799</v>
+      </c>
+      <c r="B115" t="s">
+        <v>45</v>
+      </c>
+      <c r="C115" t="s">
+        <v>397</v>
+      </c>
+      <c r="D115">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>795</v>
+      </c>
+      <c r="B116" t="s">
+        <v>90</v>
+      </c>
+      <c r="C116" t="s">
+        <v>302</v>
+      </c>
+      <c r="D116">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>797</v>
+      </c>
+      <c r="B117" t="s">
+        <v>294</v>
+      </c>
+      <c r="C117" t="s">
+        <v>303</v>
+      </c>
+      <c r="D117">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>799</v>
+      </c>
+      <c r="B118" t="s">
+        <v>90</v>
+      </c>
+      <c r="C118" t="s">
+        <v>307</v>
+      </c>
+      <c r="D118">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>798</v>
+      </c>
+      <c r="B119" t="s">
+        <v>289</v>
+      </c>
+      <c r="C119" t="s">
+        <v>306</v>
+      </c>
+      <c r="D119">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>791</v>
+      </c>
+      <c r="B120" t="s">
+        <v>187</v>
+      </c>
+      <c r="C120" t="s">
+        <v>309</v>
+      </c>
+      <c r="D120">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>790</v>
+      </c>
+      <c r="B121" t="s">
+        <v>141</v>
+      </c>
+      <c r="C121" t="s">
+        <v>312</v>
+      </c>
+      <c r="D121">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>797</v>
+      </c>
+      <c r="B122" t="s">
+        <v>313</v>
+      </c>
+      <c r="C122" t="s">
+        <v>314</v>
+      </c>
+      <c r="D122">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>794</v>
+      </c>
+      <c r="B123" t="s">
+        <v>190</v>
+      </c>
+      <c r="C123" t="s">
+        <v>315</v>
+      </c>
+      <c r="D123">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>803</v>
+      </c>
+      <c r="B124" t="s">
+        <v>98</v>
+      </c>
+      <c r="C124" t="s">
+        <v>318</v>
+      </c>
+      <c r="D124">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>793</v>
+      </c>
+      <c r="B125" t="s">
+        <v>51</v>
+      </c>
+      <c r="C125" t="s">
+        <v>319</v>
+      </c>
+      <c r="D125">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>799</v>
+      </c>
+      <c r="B126" t="s">
+        <v>126</v>
+      </c>
+      <c r="C126" t="s">
+        <v>320</v>
+      </c>
+      <c r="D126">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>790</v>
+      </c>
+      <c r="B127" t="s">
+        <v>252</v>
+      </c>
+      <c r="C127" t="s">
+        <v>321</v>
+      </c>
+      <c r="D127">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>800</v>
+      </c>
+      <c r="B128" t="s">
+        <v>328</v>
+      </c>
+      <c r="C128" t="s">
+        <v>329</v>
+      </c>
+      <c r="D128">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>799</v>
+      </c>
+      <c r="B129" t="s">
+        <v>98</v>
+      </c>
+      <c r="C129" t="s">
+        <v>323</v>
+      </c>
+      <c r="D129">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>793</v>
+      </c>
+      <c r="B130" t="s">
+        <v>98</v>
+      </c>
+      <c r="C130" t="s">
+        <v>325</v>
+      </c>
+      <c r="D130">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>799</v>
+      </c>
+      <c r="B131" t="s">
+        <v>326</v>
+      </c>
+      <c r="C131" t="s">
+        <v>327</v>
+      </c>
+      <c r="D131">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>800</v>
+      </c>
+      <c r="B132" t="s">
+        <v>35</v>
+      </c>
+      <c r="C132" t="s">
+        <v>331</v>
+      </c>
+      <c r="D132">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>801</v>
+      </c>
+      <c r="B133" t="s">
+        <v>29</v>
+      </c>
+      <c r="C133" t="s">
+        <v>332</v>
+      </c>
+      <c r="D133">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>798</v>
+      </c>
+      <c r="B134" t="s">
+        <v>35</v>
+      </c>
+      <c r="C134" t="s">
+        <v>334</v>
+      </c>
+      <c r="D134">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>798</v>
+      </c>
+      <c r="B135" t="s">
+        <v>58</v>
+      </c>
+      <c r="C135" t="s">
+        <v>335</v>
+      </c>
+      <c r="D135">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B136" t="s">
+        <v>336</v>
+      </c>
+      <c r="C136" t="s">
+        <v>337</v>
+      </c>
+      <c r="D136">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>795</v>
+      </c>
+      <c r="B137" t="s">
+        <v>339</v>
+      </c>
+      <c r="C137" t="s">
+        <v>340</v>
+      </c>
+      <c r="D137">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>799</v>
+      </c>
+      <c r="B138" t="s">
+        <v>342</v>
+      </c>
+      <c r="C138" t="s">
+        <v>274</v>
+      </c>
+      <c r="D138">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>802</v>
+      </c>
+      <c r="B139" t="s">
+        <v>183</v>
+      </c>
+      <c r="C139" t="s">
+        <v>353</v>
+      </c>
+      <c r="D139">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>793</v>
+      </c>
+      <c r="B140" t="s">
+        <v>218</v>
+      </c>
+      <c r="C140" t="s">
+        <v>343</v>
+      </c>
+      <c r="D140">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>793</v>
+      </c>
+      <c r="B141" t="s">
+        <v>54</v>
+      </c>
+      <c r="C141" t="s">
+        <v>355</v>
+      </c>
+      <c r="D141">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>797</v>
+      </c>
+      <c r="B142" t="s">
+        <v>345</v>
+      </c>
+      <c r="C142" t="s">
+        <v>346</v>
+      </c>
+      <c r="D142">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>798</v>
+      </c>
+      <c r="B143" t="s">
+        <v>104</v>
+      </c>
+      <c r="C143" t="s">
+        <v>347</v>
+      </c>
+      <c r="D143">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>802</v>
+      </c>
+      <c r="B144" t="s">
+        <v>282</v>
+      </c>
+      <c r="C144" t="s">
+        <v>349</v>
+      </c>
+      <c r="D144">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>790</v>
+      </c>
+      <c r="B145" t="s">
+        <v>351</v>
+      </c>
+      <c r="C145" t="s">
+        <v>352</v>
+      </c>
+      <c r="D145">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>791</v>
+      </c>
+      <c r="B146" t="s">
+        <v>357</v>
+      </c>
+      <c r="C146" t="s">
+        <v>358</v>
+      </c>
+      <c r="D146">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>794</v>
+      </c>
+      <c r="B147" t="s">
+        <v>218</v>
+      </c>
+      <c r="C147" t="s">
+        <v>360</v>
+      </c>
+      <c r="D147">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>792</v>
+      </c>
+      <c r="B148" t="s">
+        <v>187</v>
+      </c>
+      <c r="C148" t="s">
+        <v>361</v>
+      </c>
+      <c r="D148">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>803</v>
+      </c>
+      <c r="B149" t="s">
+        <v>362</v>
+      </c>
+      <c r="C149" t="s">
+        <v>363</v>
+      </c>
+      <c r="D149">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>803</v>
+      </c>
+      <c r="B150" t="s">
+        <v>369</v>
+      </c>
+      <c r="C150" t="s">
+        <v>370</v>
+      </c>
+      <c r="D150">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B151" t="s">
+        <v>365</v>
+      </c>
+      <c r="C151" t="s">
+        <v>366</v>
+      </c>
+      <c r="D151">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B152" t="s">
+        <v>367</v>
+      </c>
+      <c r="C152" t="s">
+        <v>368</v>
+      </c>
+      <c r="D152">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>803</v>
+      </c>
+      <c r="B153" t="s">
+        <v>215</v>
+      </c>
+      <c r="C153" t="s">
+        <v>374</v>
+      </c>
+      <c r="D153">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B154" t="s">
+        <v>98</v>
+      </c>
+      <c r="C154" t="s">
+        <v>372</v>
+      </c>
+      <c r="D154">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>792</v>
+      </c>
+      <c r="B155" t="s">
+        <v>376</v>
+      </c>
+      <c r="C155" t="s">
+        <v>377</v>
+      </c>
+      <c r="D155">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B156" t="s">
+        <v>126</v>
+      </c>
+      <c r="C156" t="s">
+        <v>379</v>
+      </c>
+      <c r="D156">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>796</v>
+      </c>
+      <c r="B157" t="s">
+        <v>289</v>
+      </c>
+      <c r="C157" t="s">
+        <v>384</v>
+      </c>
+      <c r="D157">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B158" t="s">
+        <v>339</v>
+      </c>
+      <c r="C158" t="s">
+        <v>381</v>
+      </c>
+      <c r="D158">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B159" t="s">
+        <v>187</v>
+      </c>
+      <c r="C159" t="s">
+        <v>383</v>
+      </c>
+      <c r="D159">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B160" t="s">
+        <v>58</v>
+      </c>
+      <c r="C160" t="s">
+        <v>386</v>
+      </c>
+      <c r="D160">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B161" t="s">
+        <v>388</v>
+      </c>
+      <c r="C161" t="s">
+        <v>389</v>
+      </c>
+      <c r="D161">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B162" t="s">
+        <v>390</v>
+      </c>
+      <c r="C162" t="s">
+        <v>391</v>
+      </c>
+      <c r="D162">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>795</v>
+      </c>
+      <c r="B163" t="s">
+        <v>123</v>
+      </c>
+      <c r="C163" t="s">
+        <v>392</v>
+      </c>
+      <c r="D163">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>801</v>
+      </c>
+      <c r="B164" t="s">
+        <v>282</v>
+      </c>
+      <c r="C164" t="s">
+        <v>394</v>
+      </c>
+      <c r="D164">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>794</v>
+      </c>
+      <c r="B165" t="s">
+        <v>252</v>
+      </c>
+      <c r="C165" t="s">
+        <v>253</v>
+      </c>
+      <c r="D165">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I2:L15">
+    <sortCondition ref="K2:K15"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A84FED-B2BC-46D9-8DA4-38F537BC1789}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20160,12 +22720,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B46E05-42BA-4BD3-BA0A-33215B71BBC8}">
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24439,7 +26999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A939CF14-79DD-463A-BC46-5AC1E9ABFBC5}">
   <dimension ref="A1:P165"/>
   <sheetViews>

</xml_diff>